<commit_message>
New changes for gamedetails
</commit_message>
<xml_diff>
--- a/GameNotifier/Input/Schedule.xlsx
+++ b/GameNotifier/Input/Schedule.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A287906-2BC6-46D8-B9FD-4FA88C0DE825}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8822582C-6FAA-4F03-80C2-B3DA5A3DC12E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="38">
   <si>
     <t>No.</t>
   </si>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,8 +1080,8 @@
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>32</v>
+      <c r="B22" s="8">
+        <v>43624</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
push changes to hnadling exceptions in game details
</commit_message>
<xml_diff>
--- a/GameNotifier/Input/Schedule.xlsx
+++ b/GameNotifier/Input/Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8822582C-6FAA-4F03-80C2-B3DA5A3DC12E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0009B131-8D09-4224-AD6E-331BAA96C696}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="38">
   <si>
     <t>No.</t>
   </si>
@@ -585,7 +585,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1076,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1087,11 +1087,9 @@
         <v>14</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E22" s="3"/>
       <c r="F22" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
more exceptions scenarios done
</commit_message>
<xml_diff>
--- a/GameNotifier/Input/Schedule.xlsx
+++ b/GameNotifier/Input/Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0009B131-8D09-4224-AD6E-331BAA96C696}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE47F29-2020-4982-8D39-6CDEA01C9FBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="38">
   <si>
     <t>No.</t>
   </si>
@@ -1076,7 +1076,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1089,7 +1089,9 @@
       <c r="D22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F22" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>